<commit_message>
Add auto cancel order
</commit_message>
<xml_diff>
--- a/documents/BaoCaoDot3+4/Testcase.xlsx
+++ b/documents/BaoCaoDot3+4/Testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\JavaScript\streamingmovie\documents\BaoCaoDot3+4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5782D592-AF31-47EF-8805-7432477C6C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F773AC-9276-44DB-997C-6C0E50E49073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="565">
   <si>
     <t>TÌNH TRẠNG</t>
   </si>
@@ -1982,7 +1982,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2097,7 +2097,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2115,32 +2133,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2152,10 +2149,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2571,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" topLeftCell="A260" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="H272" sqref="H272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.55" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2632,7 +2629,9 @@
         <v>270</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="5" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
@@ -2648,7 +2647,9 @@
         <v>271</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="6" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
@@ -2664,7 +2665,9 @@
         <v>260</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="7" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -2680,7 +2683,9 @@
         <v>276</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="8" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
@@ -2694,7 +2699,9 @@
         <v>279</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="9" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
@@ -2710,7 +2717,9 @@
         <v>271</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
@@ -2726,7 +2735,9 @@
         <v>281</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="11" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
@@ -2742,7 +2753,9 @@
         <v>276</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="12" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
@@ -2756,7 +2769,9 @@
         <v>285</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="13" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B13" s="15">
@@ -2772,7 +2787,9 @@
         <v>276</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="14" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -2788,7 +2805,9 @@
         <v>8</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="15" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
@@ -2814,7 +2833,9 @@
         <v>322</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
@@ -2840,7 +2861,9 @@
         <v>22</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="19" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
@@ -2856,7 +2879,9 @@
         <v>21</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="G19" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="20" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
@@ -2870,7 +2895,9 @@
         <v>14</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="21" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
@@ -2884,7 +2911,9 @@
         <v>20</v>
       </c>
       <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="G21" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="22" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
@@ -2898,7 +2927,9 @@
         <v>16</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="23" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
@@ -2914,7 +2945,9 @@
         <v>19</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="24" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
@@ -2930,7 +2963,9 @@
         <v>27</v>
       </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="25" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
@@ -2946,7 +2981,9 @@
         <v>26</v>
       </c>
       <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="26" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
@@ -2960,7 +2997,9 @@
         <v>43</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="27" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B27" s="15">
@@ -2974,7 +3013,9 @@
         <v>50</v>
       </c>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="28" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
@@ -2988,7 +3029,9 @@
         <v>51</v>
       </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="29" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B29" s="15">
@@ -3002,7 +3045,9 @@
         <v>53</v>
       </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="30" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B30" s="15">
@@ -3016,7 +3061,9 @@
         <v>76</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="31" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B31" s="15">
@@ -3030,7 +3077,9 @@
         <v>77</v>
       </c>
       <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="G31" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="32" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B32" s="15">
@@ -3046,7 +3095,9 @@
         <v>18</v>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="33" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
@@ -3072,7 +3123,9 @@
         <v>36</v>
       </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="35" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
@@ -3088,7 +3141,9 @@
         <v>31</v>
       </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="36" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
@@ -3104,7 +3159,9 @@
         <v>21</v>
       </c>
       <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
+      <c r="G36" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="37" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
@@ -3118,7 +3175,9 @@
         <v>14</v>
       </c>
       <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="38" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
@@ -3132,7 +3191,9 @@
         <v>38</v>
       </c>
       <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
+      <c r="G38" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="39" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
@@ -3148,7 +3209,9 @@
         <v>34</v>
       </c>
       <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="G39" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="40" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
@@ -3162,7 +3225,9 @@
         <v>40</v>
       </c>
       <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="41" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
@@ -3176,7 +3241,9 @@
         <v>43</v>
       </c>
       <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="42" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
@@ -3190,7 +3257,9 @@
         <v>46</v>
       </c>
       <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="G42" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="43" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B43" s="15">
@@ -3204,7 +3273,9 @@
         <v>47</v>
       </c>
       <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="44" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
@@ -3218,7 +3289,9 @@
         <v>54</v>
       </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="45" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
@@ -3232,7 +3305,9 @@
         <v>55</v>
       </c>
       <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="G45" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="46" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
@@ -3248,7 +3323,9 @@
         <v>18</v>
       </c>
       <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="47" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
@@ -3277,7 +3354,9 @@
       <c r="F48" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="49" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
@@ -3294,7 +3373,9 @@
       <c r="F49" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G49" s="4"/>
+      <c r="G49" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="50" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
@@ -3311,7 +3392,9 @@
       <c r="F50" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G50" s="4"/>
+      <c r="G50" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="51" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
@@ -3328,7 +3411,9 @@
       <c r="F51" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G51" s="4"/>
+      <c r="G51" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="52" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B52" s="3">
@@ -3345,7 +3430,9 @@
       <c r="F52" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G52" s="4"/>
+      <c r="G52" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="53" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B53" s="3">
@@ -3362,7 +3449,9 @@
       <c r="F53" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G53" s="4"/>
+      <c r="G53" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="54" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
@@ -3389,7 +3478,9 @@
         <v>73</v>
       </c>
       <c r="F55" s="13"/>
-      <c r="G55" s="4"/>
+      <c r="G55" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="56" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B56" s="3">
@@ -3406,7 +3497,9 @@
         <v>79</v>
       </c>
       <c r="F56" s="13"/>
-      <c r="G56" s="4"/>
+      <c r="G56" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="57" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B57" s="3">
@@ -3423,7 +3516,9 @@
         <v>81</v>
       </c>
       <c r="F57" s="13"/>
-      <c r="G57" s="4"/>
+      <c r="G57" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="58" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
@@ -3440,7 +3535,9 @@
         <v>83</v>
       </c>
       <c r="F58" s="13"/>
-      <c r="G58" s="4"/>
+      <c r="G58" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="59" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B59" s="3">
@@ -3457,7 +3554,9 @@
         <v>86</v>
       </c>
       <c r="F59" s="13"/>
-      <c r="G59" s="4"/>
+      <c r="G59" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="60" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B60" s="3">
@@ -3472,7 +3571,9 @@
         <v>87</v>
       </c>
       <c r="F60" s="13"/>
-      <c r="G60" s="4"/>
+      <c r="G60" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="61" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B61" s="3">
@@ -3489,7 +3590,9 @@
       <c r="F61" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G61" s="4"/>
+      <c r="G61" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="62" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B62" s="3">
@@ -3504,7 +3607,9 @@
         <v>98</v>
       </c>
       <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
+      <c r="G62" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="63" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B63" s="3">
@@ -3519,7 +3624,9 @@
         <v>62</v>
       </c>
       <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
+      <c r="G63" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="64" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B64" s="3">
@@ -3536,7 +3643,9 @@
       <c r="F64" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G64" s="4"/>
+      <c r="G64" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="65" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B65" s="3">
@@ -3551,7 +3660,9 @@
         <v>96</v>
       </c>
       <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
+      <c r="G65" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="66" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B66" s="3">
@@ -3566,7 +3677,9 @@
         <v>62</v>
       </c>
       <c r="F66" s="13"/>
-      <c r="G66" s="4"/>
+      <c r="G66" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="67" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B67" s="3">
@@ -3581,7 +3694,9 @@
         <v>93</v>
       </c>
       <c r="F67" s="13"/>
-      <c r="G67" s="4"/>
+      <c r="G67" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="68" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B68" s="3">
@@ -3596,7 +3711,9 @@
         <v>101</v>
       </c>
       <c r="F68" s="13"/>
-      <c r="G68" s="4"/>
+      <c r="G68" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="69" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B69" s="3">
@@ -3611,7 +3728,9 @@
         <v>103</v>
       </c>
       <c r="F69" s="13"/>
-      <c r="G69" s="4"/>
+      <c r="G69" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="70" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B70" s="3">
@@ -3626,7 +3745,9 @@
         <v>128</v>
       </c>
       <c r="F70" s="13"/>
-      <c r="G70" s="4"/>
+      <c r="G70" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="71" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
@@ -3666,7 +3787,9 @@
         <v>73</v>
       </c>
       <c r="F73" s="13"/>
-      <c r="G73" s="4"/>
+      <c r="G73" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="74" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="str">
@@ -3683,7 +3806,9 @@
         <v>79</v>
       </c>
       <c r="F74" s="13"/>
-      <c r="G74" s="4"/>
+      <c r="G74" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="75" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="str">
@@ -3700,7 +3825,9 @@
         <v>81</v>
       </c>
       <c r="F75" s="13"/>
-      <c r="G75" s="4"/>
+      <c r="G75" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="76" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="str">
@@ -3717,7 +3844,9 @@
         <v>104</v>
       </c>
       <c r="F76" s="13"/>
-      <c r="G76" s="4"/>
+      <c r="G76" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="77" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="str">
@@ -3732,7 +3861,9 @@
         <v>106</v>
       </c>
       <c r="F77" s="13"/>
-      <c r="G77" s="4"/>
+      <c r="G77" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="78" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="str">
@@ -3747,7 +3878,9 @@
         <v>116</v>
       </c>
       <c r="F78" s="13"/>
-      <c r="G78" s="4"/>
+      <c r="G78" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="79" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="str">
@@ -3792,7 +3925,9 @@
         <v>112</v>
       </c>
       <c r="F81" s="13"/>
-      <c r="G81" s="4"/>
+      <c r="G81" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="82" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="str">
@@ -3807,7 +3942,9 @@
         <v>114</v>
       </c>
       <c r="F82" s="13"/>
-      <c r="G82" s="4"/>
+      <c r="G82" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="83" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="str">
@@ -3822,7 +3959,9 @@
         <v>118</v>
       </c>
       <c r="F83" s="13"/>
-      <c r="G83" s="4"/>
+      <c r="G83" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="84" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="str">
@@ -3837,7 +3976,9 @@
         <v>114</v>
       </c>
       <c r="F84" s="13"/>
-      <c r="G84" s="4"/>
+      <c r="G84" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="85" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="str">
@@ -3852,7 +3993,9 @@
         <v>121</v>
       </c>
       <c r="F85" s="13"/>
-      <c r="G85" s="4"/>
+      <c r="G85" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="86" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="str">
@@ -3867,7 +4010,9 @@
         <v>121</v>
       </c>
       <c r="F86" s="13"/>
-      <c r="G86" s="4"/>
+      <c r="G86" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="87" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="str">
@@ -3882,7 +4027,9 @@
         <v>123</v>
       </c>
       <c r="F87" s="13"/>
-      <c r="G87" s="4"/>
+      <c r="G87" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="88" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="str">
@@ -3927,7 +4074,9 @@
         <v>131</v>
       </c>
       <c r="F90" s="13"/>
-      <c r="G90" s="4"/>
+      <c r="G90" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="91" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="str">
@@ -3942,7 +4091,9 @@
         <v>133</v>
       </c>
       <c r="F91" s="13"/>
-      <c r="G91" s="4"/>
+      <c r="G91" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="92" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="str">
@@ -3957,7 +4108,9 @@
         <v>134</v>
       </c>
       <c r="F92" s="13"/>
-      <c r="G92" s="4"/>
+      <c r="G92" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="93" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="str">
@@ -3972,7 +4125,9 @@
         <v>40</v>
       </c>
       <c r="F93" s="13"/>
-      <c r="G93" s="4"/>
+      <c r="G93" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="94" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="str">
@@ -3987,7 +4142,9 @@
         <v>40</v>
       </c>
       <c r="F94" s="13"/>
-      <c r="G94" s="4"/>
+      <c r="G94" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="95" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="str">
@@ -4002,7 +4159,9 @@
         <v>137</v>
       </c>
       <c r="F95" s="13"/>
-      <c r="G95" s="4"/>
+      <c r="G95" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="96" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="str">
@@ -4017,7 +4176,9 @@
         <v>140</v>
       </c>
       <c r="F96" s="13"/>
-      <c r="G96" s="4"/>
+      <c r="G96" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="97" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="str">
@@ -4032,7 +4193,9 @@
         <v>123</v>
       </c>
       <c r="F97" s="13"/>
-      <c r="G97" s="4"/>
+      <c r="G97" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="98" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="str">
@@ -4068,7 +4231,7 @@
         <f>B99 + 0.1</f>
         <v>8.1</v>
       </c>
-      <c r="C100" s="46" t="s">
+      <c r="C100" s="51" t="s">
         <v>324</v>
       </c>
       <c r="D100" s="17" t="s">
@@ -4078,14 +4241,16 @@
         <v>325</v>
       </c>
       <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="G100" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="101" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B101" s="3">
         <f t="shared" ref="B101:B108" si="3">B100 + 0.1</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="C101" s="47"/>
+      <c r="C101" s="53"/>
       <c r="D101" s="17" t="s">
         <v>332</v>
       </c>
@@ -4093,7 +4258,9 @@
         <v>331</v>
       </c>
       <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
+      <c r="G101" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="102" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B102" s="3">
@@ -4108,7 +4275,9 @@
         <v>327</v>
       </c>
       <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
+      <c r="G102" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="103" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B103" s="3">
@@ -4125,14 +4294,16 @@
         <v>329</v>
       </c>
       <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
+      <c r="G103" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="104" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B104" s="3">
         <f t="shared" si="3"/>
         <v>8.4999999999999982</v>
       </c>
-      <c r="C104" s="65" t="s">
+      <c r="C104" s="46" t="s">
         <v>564</v>
       </c>
       <c r="D104" s="4" t="s">
@@ -4142,7 +4313,9 @@
         <v>563</v>
       </c>
       <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
+      <c r="G104" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="105" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B105" s="3">
@@ -4157,7 +4330,9 @@
         <v>334</v>
       </c>
       <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
+      <c r="G105" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="106" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B106" s="3">
@@ -4174,7 +4349,9 @@
         <v>337</v>
       </c>
       <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
+      <c r="G106" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="107" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B107" s="3">
@@ -4189,7 +4366,9 @@
         <v>325</v>
       </c>
       <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
+      <c r="G107" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="108" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B108" s="3">
@@ -4233,7 +4412,9 @@
         <v>147</v>
       </c>
       <c r="F110" s="13"/>
-      <c r="G110" s="4"/>
+      <c r="G110" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="111" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B111" s="3">
@@ -4250,7 +4431,9 @@
       <c r="F111" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="G111" s="4"/>
+      <c r="G111" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="112" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B112" s="3">
@@ -4267,7 +4450,9 @@
         <v>153</v>
       </c>
       <c r="F112" s="13"/>
-      <c r="G112" s="4"/>
+      <c r="G112" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="113" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B113" s="3">
@@ -4284,14 +4469,16 @@
         <v>157</v>
       </c>
       <c r="F113" s="13"/>
-      <c r="G113" s="4"/>
+      <c r="G113" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="114" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B114" s="3">
         <f t="shared" si="4"/>
         <v>9.4999999999999982</v>
       </c>
-      <c r="C114" s="54" t="s">
+      <c r="C114" s="47" t="s">
         <v>160</v>
       </c>
       <c r="D114" s="17" t="s">
@@ -4301,14 +4488,16 @@
         <v>208</v>
       </c>
       <c r="F114" s="13"/>
-      <c r="G114" s="48"/>
+      <c r="G114" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="115" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B115" s="3">
         <f t="shared" si="4"/>
         <v>9.5999999999999979</v>
       </c>
-      <c r="C115" s="55"/>
+      <c r="C115" s="48"/>
       <c r="D115" s="17" t="s">
         <v>162</v>
       </c>
@@ -4316,14 +4505,14 @@
         <v>208</v>
       </c>
       <c r="F115" s="13"/>
-      <c r="G115" s="49"/>
+      <c r="G115" s="52"/>
     </row>
     <row r="116" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B116" s="3">
         <f t="shared" si="4"/>
         <v>9.6999999999999975</v>
       </c>
-      <c r="C116" s="56"/>
+      <c r="C116" s="49"/>
       <c r="D116" s="17" t="s">
         <v>163</v>
       </c>
@@ -4331,14 +4520,14 @@
         <v>209</v>
       </c>
       <c r="F116" s="13"/>
-      <c r="G116" s="50"/>
+      <c r="G116" s="53"/>
     </row>
     <row r="117" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B117" s="3">
         <f t="shared" si="4"/>
         <v>9.7999999999999972</v>
       </c>
-      <c r="C117" s="64" t="s">
+      <c r="C117" s="50" t="s">
         <v>159</v>
       </c>
       <c r="D117" s="17" t="s">
@@ -4348,14 +4537,16 @@
         <v>202</v>
       </c>
       <c r="F117" s="13"/>
-      <c r="G117" s="48"/>
+      <c r="G117" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="118" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B118" s="3">
         <f t="shared" si="4"/>
         <v>9.8999999999999968</v>
       </c>
-      <c r="C118" s="64"/>
+      <c r="C118" s="50"/>
       <c r="D118" s="17" t="s">
         <v>165</v>
       </c>
@@ -4363,14 +4554,14 @@
         <v>203</v>
       </c>
       <c r="F118" s="13"/>
-      <c r="G118" s="49"/>
+      <c r="G118" s="52"/>
     </row>
     <row r="119" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B119" s="15">
         <f>B110</f>
         <v>9.1</v>
       </c>
-      <c r="C119" s="64"/>
+      <c r="C119" s="50"/>
       <c r="D119" s="17" t="s">
         <v>166</v>
       </c>
@@ -4378,14 +4569,14 @@
         <v>204</v>
       </c>
       <c r="F119" s="13"/>
-      <c r="G119" s="49"/>
+      <c r="G119" s="52"/>
     </row>
     <row r="120" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B120" s="15">
         <f>B119+0.01</f>
         <v>9.11</v>
       </c>
-      <c r="C120" s="64"/>
+      <c r="C120" s="50"/>
       <c r="D120" s="17" t="s">
         <v>168</v>
       </c>
@@ -4393,14 +4584,14 @@
         <v>205</v>
       </c>
       <c r="F120" s="13"/>
-      <c r="G120" s="50"/>
+      <c r="G120" s="53"/>
     </row>
     <row r="121" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B121" s="15">
         <f t="shared" ref="B121:B123" si="5">B120+0.01</f>
         <v>9.1199999999999992</v>
       </c>
-      <c r="C121" s="46" t="s">
+      <c r="C121" s="51" t="s">
         <v>158</v>
       </c>
       <c r="D121" s="17" t="s">
@@ -4410,14 +4601,16 @@
         <v>206</v>
       </c>
       <c r="F121" s="13"/>
-      <c r="G121" s="48"/>
+      <c r="G121" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="122" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B122" s="15">
         <f t="shared" si="5"/>
         <v>9.129999999999999</v>
       </c>
-      <c r="C122" s="60"/>
+      <c r="C122" s="52"/>
       <c r="D122" s="17" t="s">
         <v>170</v>
       </c>
@@ -4425,14 +4618,14 @@
         <v>206</v>
       </c>
       <c r="F122" s="13"/>
-      <c r="G122" s="49"/>
+      <c r="G122" s="52"/>
     </row>
     <row r="123" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B123" s="15">
         <f t="shared" si="5"/>
         <v>9.1399999999999988</v>
       </c>
-      <c r="C123" s="47"/>
+      <c r="C123" s="53"/>
       <c r="D123" s="17" t="s">
         <v>171</v>
       </c>
@@ -4440,101 +4633,105 @@
         <v>207</v>
       </c>
       <c r="F123" s="13"/>
-      <c r="G123" s="50"/>
+      <c r="G123" s="53"/>
     </row>
     <row r="124" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B124" s="61">
+      <c r="B124" s="60">
         <f>B123+0.01</f>
         <v>9.1499999999999986</v>
       </c>
-      <c r="C124" s="54" t="s">
+      <c r="C124" s="47" t="s">
         <v>230</v>
       </c>
       <c r="D124" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E124" s="46" t="s">
+      <c r="E124" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="F124" s="51"/>
-      <c r="G124" s="48"/>
+      <c r="F124" s="57"/>
+      <c r="G124" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="125" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B125" s="62"/>
-      <c r="C125" s="55"/>
+      <c r="B125" s="61"/>
+      <c r="C125" s="48"/>
       <c r="D125" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E125" s="60"/>
-      <c r="F125" s="57"/>
-      <c r="G125" s="49"/>
+      <c r="E125" s="52"/>
+      <c r="F125" s="58"/>
+      <c r="G125" s="52"/>
     </row>
     <row r="126" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B126" s="62"/>
-      <c r="C126" s="55"/>
+      <c r="B126" s="61"/>
+      <c r="C126" s="48"/>
       <c r="D126" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E126" s="60"/>
-      <c r="F126" s="57"/>
-      <c r="G126" s="49"/>
+      <c r="E126" s="52"/>
+      <c r="F126" s="58"/>
+      <c r="G126" s="52"/>
     </row>
     <row r="127" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B127" s="63"/>
-      <c r="C127" s="56"/>
+      <c r="B127" s="62"/>
+      <c r="C127" s="49"/>
       <c r="D127" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E127" s="47"/>
-      <c r="F127" s="52"/>
-      <c r="G127" s="50"/>
+      <c r="E127" s="53"/>
+      <c r="F127" s="59"/>
+      <c r="G127" s="53"/>
     </row>
     <row r="128" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B128" s="61">
+      <c r="B128" s="60">
         <f>B124+0.01</f>
         <v>9.1599999999999984</v>
       </c>
-      <c r="C128" s="54" t="s">
+      <c r="C128" s="47" t="s">
         <v>229</v>
       </c>
       <c r="D128" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E128" s="46" t="s">
+      <c r="E128" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="F128" s="51"/>
-      <c r="G128" s="48"/>
+      <c r="F128" s="57"/>
+      <c r="G128" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="129" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B129" s="62"/>
-      <c r="C129" s="55"/>
+      <c r="B129" s="61"/>
+      <c r="C129" s="48"/>
       <c r="D129" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E129" s="60"/>
-      <c r="F129" s="57"/>
-      <c r="G129" s="49"/>
+      <c r="E129" s="52"/>
+      <c r="F129" s="58"/>
+      <c r="G129" s="52"/>
     </row>
     <row r="130" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B130" s="62"/>
-      <c r="C130" s="55"/>
+      <c r="B130" s="61"/>
+      <c r="C130" s="48"/>
       <c r="D130" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E130" s="60"/>
-      <c r="F130" s="57"/>
-      <c r="G130" s="49"/>
+      <c r="E130" s="52"/>
+      <c r="F130" s="58"/>
+      <c r="G130" s="52"/>
     </row>
     <row r="131" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B131" s="63"/>
-      <c r="C131" s="56"/>
+      <c r="B131" s="62"/>
+      <c r="C131" s="49"/>
       <c r="D131" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="E131" s="47"/>
-      <c r="F131" s="52"/>
-      <c r="G131" s="50"/>
+      <c r="E131" s="53"/>
+      <c r="F131" s="59"/>
+      <c r="G131" s="53"/>
     </row>
     <row r="132" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B132" s="15">
@@ -4549,7 +4746,9 @@
         <v>249</v>
       </c>
       <c r="F132" s="13"/>
-      <c r="G132" s="4"/>
+      <c r="G132" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="133" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B133" s="15">
@@ -4566,7 +4765,9 @@
         <v>8</v>
       </c>
       <c r="F133" s="13"/>
-      <c r="G133" s="4"/>
+      <c r="G133" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="134" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B134" s="2">
@@ -4593,7 +4794,9 @@
         <v>173</v>
       </c>
       <c r="F135" s="13"/>
-      <c r="G135" s="4"/>
+      <c r="G135" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="136" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B136" s="3">
@@ -4608,7 +4811,9 @@
         <v>175</v>
       </c>
       <c r="F136" s="13"/>
-      <c r="G136" s="4"/>
+      <c r="G136" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="137" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B137" s="3">
@@ -4625,7 +4830,9 @@
         <v>210</v>
       </c>
       <c r="F137" s="13"/>
-      <c r="G137" s="4"/>
+      <c r="G137" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="138" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B138" s="3">
@@ -4642,14 +4849,16 @@
         <v>211</v>
       </c>
       <c r="F138" s="13"/>
-      <c r="G138" s="4"/>
+      <c r="G138" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="139" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B139" s="3">
         <f t="shared" si="6"/>
         <v>10.499999999999998</v>
       </c>
-      <c r="C139" s="46" t="s">
+      <c r="C139" s="51" t="s">
         <v>160</v>
       </c>
       <c r="D139" s="17" t="s">
@@ -4659,14 +4868,16 @@
         <v>208</v>
       </c>
       <c r="F139" s="13"/>
-      <c r="G139" s="48"/>
+      <c r="G139" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="140" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B140" s="3">
         <f t="shared" si="6"/>
         <v>10.599999999999998</v>
       </c>
-      <c r="C140" s="60"/>
+      <c r="C140" s="52"/>
       <c r="D140" s="17" t="s">
         <v>183</v>
       </c>
@@ -4674,14 +4885,14 @@
         <v>208</v>
       </c>
       <c r="F140" s="13"/>
-      <c r="G140" s="49"/>
+      <c r="G140" s="52"/>
     </row>
     <row r="141" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B141" s="3">
         <f t="shared" si="6"/>
         <v>10.699999999999998</v>
       </c>
-      <c r="C141" s="47"/>
+      <c r="C141" s="53"/>
       <c r="D141" s="17" t="s">
         <v>184</v>
       </c>
@@ -4689,14 +4900,14 @@
         <v>208</v>
       </c>
       <c r="F141" s="13"/>
-      <c r="G141" s="50"/>
+      <c r="G141" s="53"/>
     </row>
     <row r="142" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B142" s="3">
         <f t="shared" si="6"/>
         <v>10.799999999999997</v>
       </c>
-      <c r="C142" s="46" t="s">
+      <c r="C142" s="51" t="s">
         <v>159</v>
       </c>
       <c r="D142" s="17" t="s">
@@ -4706,14 +4917,16 @@
         <v>212</v>
       </c>
       <c r="F142" s="13"/>
-      <c r="G142" s="48"/>
+      <c r="G142" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="143" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B143" s="3">
         <f t="shared" si="6"/>
         <v>10.899999999999997</v>
       </c>
-      <c r="C143" s="60"/>
+      <c r="C143" s="52"/>
       <c r="D143" s="17" t="s">
         <v>185</v>
       </c>
@@ -4721,14 +4934,14 @@
         <v>213</v>
       </c>
       <c r="F143" s="13"/>
-      <c r="G143" s="49"/>
+      <c r="G143" s="52"/>
     </row>
     <row r="144" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B144" s="15">
         <f>B135</f>
         <v>10.1</v>
       </c>
-      <c r="C144" s="60"/>
+      <c r="C144" s="52"/>
       <c r="D144" s="17" t="s">
         <v>166</v>
       </c>
@@ -4736,14 +4949,14 @@
         <v>204</v>
       </c>
       <c r="F144" s="13"/>
-      <c r="G144" s="49"/>
+      <c r="G144" s="52"/>
     </row>
     <row r="145" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B145" s="15">
         <f>B144+0.01</f>
         <v>10.11</v>
       </c>
-      <c r="C145" s="47"/>
+      <c r="C145" s="53"/>
       <c r="D145" s="17" t="s">
         <v>168</v>
       </c>
@@ -4751,14 +4964,14 @@
         <v>205</v>
       </c>
       <c r="F145" s="13"/>
-      <c r="G145" s="50"/>
+      <c r="G145" s="53"/>
     </row>
     <row r="146" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B146" s="15">
         <f t="shared" ref="B146:B149" si="7">B145+0.01</f>
         <v>10.119999999999999</v>
       </c>
-      <c r="C146" s="46" t="s">
+      <c r="C146" s="51" t="s">
         <v>158</v>
       </c>
       <c r="D146" s="17" t="s">
@@ -4768,14 +4981,16 @@
         <v>206</v>
       </c>
       <c r="F146" s="13"/>
-      <c r="G146" s="48"/>
+      <c r="G146" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="147" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B147" s="15">
         <f t="shared" si="7"/>
         <v>10.129999999999999</v>
       </c>
-      <c r="C147" s="60"/>
+      <c r="C147" s="52"/>
       <c r="D147" s="17" t="s">
         <v>170</v>
       </c>
@@ -4783,14 +4998,14 @@
         <v>206</v>
       </c>
       <c r="F147" s="13"/>
-      <c r="G147" s="49"/>
+      <c r="G147" s="52"/>
     </row>
     <row r="148" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B148" s="15">
         <f t="shared" si="7"/>
         <v>10.139999999999999</v>
       </c>
-      <c r="C148" s="47"/>
+      <c r="C148" s="53"/>
       <c r="D148" s="17" t="s">
         <v>171</v>
       </c>
@@ -4798,101 +5013,105 @@
         <v>214</v>
       </c>
       <c r="F148" s="13"/>
-      <c r="G148" s="50"/>
+      <c r="G148" s="53"/>
     </row>
     <row r="149" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B149" s="61">
+      <c r="B149" s="60">
         <f t="shared" si="7"/>
         <v>10.149999999999999</v>
       </c>
-      <c r="C149" s="54" t="s">
+      <c r="C149" s="47" t="s">
         <v>230</v>
       </c>
       <c r="D149" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E149" s="46" t="s">
+      <c r="E149" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="F149" s="51"/>
-      <c r="G149" s="48"/>
+      <c r="F149" s="57"/>
+      <c r="G149" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="150" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B150" s="62"/>
-      <c r="C150" s="55"/>
+      <c r="B150" s="61"/>
+      <c r="C150" s="48"/>
       <c r="D150" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E150" s="60"/>
-      <c r="F150" s="57"/>
-      <c r="G150" s="49"/>
+      <c r="E150" s="52"/>
+      <c r="F150" s="58"/>
+      <c r="G150" s="52"/>
     </row>
     <row r="151" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B151" s="62"/>
-      <c r="C151" s="55"/>
+      <c r="B151" s="61"/>
+      <c r="C151" s="48"/>
       <c r="D151" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E151" s="60"/>
-      <c r="F151" s="57"/>
-      <c r="G151" s="49"/>
+      <c r="E151" s="52"/>
+      <c r="F151" s="58"/>
+      <c r="G151" s="52"/>
     </row>
     <row r="152" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B152" s="63"/>
-      <c r="C152" s="56"/>
+      <c r="B152" s="62"/>
+      <c r="C152" s="49"/>
       <c r="D152" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E152" s="47"/>
-      <c r="F152" s="52"/>
-      <c r="G152" s="50"/>
+      <c r="E152" s="53"/>
+      <c r="F152" s="59"/>
+      <c r="G152" s="53"/>
     </row>
     <row r="153" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B153" s="61">
+      <c r="B153" s="60">
         <f>B149+0.01</f>
         <v>10.159999999999998</v>
       </c>
-      <c r="C153" s="54" t="s">
+      <c r="C153" s="47" t="s">
         <v>229</v>
       </c>
       <c r="D153" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E153" s="46" t="s">
+      <c r="E153" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="F153" s="51"/>
-      <c r="G153" s="48"/>
+      <c r="F153" s="57"/>
+      <c r="G153" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="154" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B154" s="49"/>
-      <c r="C154" s="55"/>
+      <c r="B154" s="55"/>
+      <c r="C154" s="48"/>
       <c r="D154" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E154" s="60"/>
-      <c r="F154" s="57"/>
-      <c r="G154" s="49"/>
+      <c r="E154" s="52"/>
+      <c r="F154" s="58"/>
+      <c r="G154" s="52"/>
     </row>
     <row r="155" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B155" s="49"/>
-      <c r="C155" s="55"/>
+      <c r="B155" s="55"/>
+      <c r="C155" s="48"/>
       <c r="D155" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E155" s="60"/>
-      <c r="F155" s="57"/>
-      <c r="G155" s="49"/>
+      <c r="E155" s="52"/>
+      <c r="F155" s="58"/>
+      <c r="G155" s="52"/>
     </row>
     <row r="156" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B156" s="50"/>
-      <c r="C156" s="56"/>
+      <c r="B156" s="56"/>
+      <c r="C156" s="49"/>
       <c r="D156" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="E156" s="47"/>
-      <c r="F156" s="52"/>
-      <c r="G156" s="50"/>
+      <c r="E156" s="53"/>
+      <c r="F156" s="59"/>
+      <c r="G156" s="53"/>
     </row>
     <row r="157" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B157" s="15">
@@ -4909,7 +5128,9 @@
         <v>8</v>
       </c>
       <c r="F157" s="13"/>
-      <c r="G157" s="4"/>
+      <c r="G157" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="158" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B158" s="2">
@@ -4938,7 +5159,9 @@
       <c r="F159" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="G159" s="4"/>
+      <c r="G159" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="160" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B160" s="3">
@@ -4957,7 +5180,9 @@
       <c r="F160" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="G160" s="4"/>
+      <c r="G160" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="161" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B161" s="3">
@@ -4976,46 +5201,50 @@
       <c r="F161" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="G161" s="18"/>
+      <c r="G161" s="18" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="162" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
-      <c r="B162" s="48">
+      <c r="B162" s="54">
         <f>B161+0.1</f>
         <v>11.299999999999999</v>
       </c>
-      <c r="C162" s="46" t="s">
+      <c r="C162" s="51" t="s">
         <v>192</v>
       </c>
       <c r="D162" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E162" s="46" t="s">
+      <c r="E162" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="F162" s="54" t="s">
+      <c r="F162" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="G162" s="48"/>
+      <c r="G162" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="163" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
-      <c r="B163" s="49"/>
-      <c r="C163" s="60"/>
+      <c r="B163" s="55"/>
+      <c r="C163" s="52"/>
       <c r="D163" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E163" s="60"/>
-      <c r="F163" s="55"/>
-      <c r="G163" s="49"/>
+      <c r="E163" s="52"/>
+      <c r="F163" s="48"/>
+      <c r="G163" s="52"/>
     </row>
     <row r="164" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
-      <c r="B164" s="50"/>
-      <c r="C164" s="47"/>
+      <c r="B164" s="56"/>
+      <c r="C164" s="53"/>
       <c r="D164" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="E164" s="47"/>
-      <c r="F164" s="56"/>
-      <c r="G164" s="50"/>
+      <c r="E164" s="53"/>
+      <c r="F164" s="49"/>
+      <c r="G164" s="53"/>
     </row>
     <row r="165" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B165" s="3">
@@ -5034,158 +5263,166 @@
       <c r="F165" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="G165" s="4"/>
+      <c r="G165" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="166" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
-      <c r="B166" s="48">
+      <c r="B166" s="54">
         <f>B165+0.1</f>
         <v>11.499999999999998</v>
       </c>
-      <c r="C166" s="46" t="s">
+      <c r="C166" s="51" t="s">
         <v>219</v>
       </c>
       <c r="D166" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="E166" s="46" t="s">
+      <c r="E166" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="F166" s="51"/>
-      <c r="G166" s="48"/>
+      <c r="F166" s="57"/>
+      <c r="G166" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="167" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B167" s="49"/>
-      <c r="C167" s="60"/>
+      <c r="B167" s="55"/>
+      <c r="C167" s="52"/>
       <c r="D167" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E167" s="60"/>
-      <c r="F167" s="57"/>
-      <c r="G167" s="49"/>
+      <c r="E167" s="52"/>
+      <c r="F167" s="58"/>
+      <c r="G167" s="52"/>
     </row>
     <row r="168" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B168" s="49"/>
-      <c r="C168" s="60"/>
+      <c r="B168" s="55"/>
+      <c r="C168" s="52"/>
       <c r="D168" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E168" s="60"/>
-      <c r="F168" s="57"/>
-      <c r="G168" s="49"/>
+      <c r="E168" s="52"/>
+      <c r="F168" s="58"/>
+      <c r="G168" s="52"/>
     </row>
     <row r="169" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
-      <c r="B169" s="50"/>
-      <c r="C169" s="47"/>
+      <c r="B169" s="56"/>
+      <c r="C169" s="53"/>
       <c r="D169" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="E169" s="47"/>
-      <c r="F169" s="52"/>
-      <c r="G169" s="50"/>
+      <c r="E169" s="53"/>
+      <c r="F169" s="59"/>
+      <c r="G169" s="53"/>
     </row>
     <row r="170" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B170" s="48">
+      <c r="B170" s="54">
         <f>B166+0.1</f>
         <v>11.599999999999998</v>
       </c>
-      <c r="C170" s="46" t="s">
+      <c r="C170" s="51" t="s">
         <v>231</v>
       </c>
       <c r="D170" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E170" s="54" t="s">
+      <c r="E170" s="47" t="s">
         <v>234</v>
       </c>
-      <c r="F170" s="51"/>
-      <c r="G170" s="48"/>
+      <c r="F170" s="57"/>
+      <c r="G170" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="171" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B171" s="49"/>
-      <c r="C171" s="60"/>
+      <c r="B171" s="55"/>
+      <c r="C171" s="52"/>
       <c r="D171" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E171" s="55"/>
-      <c r="F171" s="57"/>
-      <c r="G171" s="49"/>
+      <c r="E171" s="48"/>
+      <c r="F171" s="58"/>
+      <c r="G171" s="52"/>
     </row>
     <row r="172" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B172" s="49"/>
-      <c r="C172" s="60"/>
+      <c r="B172" s="55"/>
+      <c r="C172" s="52"/>
       <c r="D172" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="E172" s="55"/>
-      <c r="F172" s="57"/>
-      <c r="G172" s="49"/>
+      <c r="E172" s="48"/>
+      <c r="F172" s="58"/>
+      <c r="G172" s="52"/>
     </row>
     <row r="173" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B173" s="50"/>
-      <c r="C173" s="47"/>
+      <c r="B173" s="56"/>
+      <c r="C173" s="53"/>
       <c r="D173" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E173" s="56"/>
-      <c r="F173" s="52"/>
-      <c r="G173" s="50"/>
+      <c r="E173" s="49"/>
+      <c r="F173" s="59"/>
+      <c r="G173" s="53"/>
     </row>
     <row r="174" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B174" s="48">
+      <c r="B174" s="54">
         <f>B170+0.1</f>
         <v>11.699999999999998</v>
       </c>
-      <c r="C174" s="58" t="s">
+      <c r="C174" s="63" t="s">
         <v>235</v>
       </c>
       <c r="D174" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="E174" s="58" t="s">
+      <c r="E174" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="F174" s="59"/>
-      <c r="G174" s="53"/>
+      <c r="F174" s="64"/>
+      <c r="G174" s="50" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="175" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B175" s="49"/>
-      <c r="C175" s="58"/>
+      <c r="B175" s="55"/>
+      <c r="C175" s="63"/>
       <c r="D175" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="E175" s="58"/>
-      <c r="F175" s="59"/>
-      <c r="G175" s="53"/>
+      <c r="E175" s="63"/>
+      <c r="F175" s="64"/>
+      <c r="G175" s="50"/>
     </row>
     <row r="176" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B176" s="49"/>
-      <c r="C176" s="58"/>
+      <c r="B176" s="55"/>
+      <c r="C176" s="63"/>
       <c r="D176" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="E176" s="58"/>
-      <c r="F176" s="59"/>
-      <c r="G176" s="53"/>
+      <c r="E176" s="63"/>
+      <c r="F176" s="64"/>
+      <c r="G176" s="50"/>
     </row>
     <row r="177" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B177" s="49"/>
-      <c r="C177" s="58"/>
+      <c r="B177" s="55"/>
+      <c r="C177" s="63"/>
       <c r="D177" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="E177" s="58"/>
-      <c r="F177" s="59"/>
-      <c r="G177" s="53"/>
+      <c r="E177" s="63"/>
+      <c r="F177" s="64"/>
+      <c r="G177" s="50"/>
     </row>
     <row r="178" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B178" s="50"/>
-      <c r="C178" s="58"/>
+      <c r="B178" s="56"/>
+      <c r="C178" s="63"/>
       <c r="D178" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="E178" s="58"/>
-      <c r="F178" s="59"/>
-      <c r="G178" s="53"/>
+      <c r="E178" s="63"/>
+      <c r="F178" s="64"/>
+      <c r="G178" s="50"/>
     </row>
     <row r="179" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B179" s="3">
@@ -5200,14 +5437,16 @@
         <v>239</v>
       </c>
       <c r="F179" s="13"/>
-      <c r="G179" s="4"/>
+      <c r="G179" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="180" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B180" s="3">
         <f>B179+0.1</f>
         <v>11.899999999999997</v>
       </c>
-      <c r="C180" s="46" t="s">
+      <c r="C180" s="51" t="s">
         <v>178</v>
       </c>
       <c r="D180" s="17" t="s">
@@ -5217,14 +5456,16 @@
         <v>180</v>
       </c>
       <c r="F180" s="13"/>
-      <c r="G180" s="4"/>
+      <c r="G180" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="181" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B181" s="15">
         <f>B160</f>
         <v>11.1</v>
       </c>
-      <c r="C181" s="47"/>
+      <c r="C181" s="53"/>
       <c r="D181" s="17" t="s">
         <v>181</v>
       </c>
@@ -5232,7 +5473,9 @@
         <v>182</v>
       </c>
       <c r="F181" s="13"/>
-      <c r="G181" s="4"/>
+      <c r="G181" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="182" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B182" s="15">
@@ -5247,7 +5490,9 @@
         <v>241</v>
       </c>
       <c r="F182" s="13"/>
-      <c r="G182" s="4"/>
+      <c r="G182" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="183" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B183" s="2">
@@ -5274,7 +5519,9 @@
         <v>341</v>
       </c>
       <c r="F184" s="13"/>
-      <c r="G184" s="4"/>
+      <c r="G184" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="185" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B185" s="3">
@@ -5289,7 +5536,9 @@
         <v>343</v>
       </c>
       <c r="F185" s="13"/>
-      <c r="G185" s="4"/>
+      <c r="G185" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="186" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B186" s="3">
@@ -5304,7 +5553,9 @@
         <v>345</v>
       </c>
       <c r="F186" s="13"/>
-      <c r="G186" s="4"/>
+      <c r="G186" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="187" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B187" s="3">
@@ -5321,7 +5572,9 @@
         <v>348</v>
       </c>
       <c r="F187" s="13"/>
-      <c r="G187" s="4"/>
+      <c r="G187" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="188" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B188" s="3">
@@ -5338,7 +5591,9 @@
         <v>353</v>
       </c>
       <c r="F188" s="13"/>
-      <c r="G188" s="4"/>
+      <c r="G188" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="189" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B189" s="3">
@@ -5355,7 +5610,9 @@
         <v>354</v>
       </c>
       <c r="F189" s="13"/>
-      <c r="G189" s="4"/>
+      <c r="G189" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="190" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B190" s="3">
@@ -5370,7 +5627,9 @@
         <v>359</v>
       </c>
       <c r="F190" s="13"/>
-      <c r="G190" s="4"/>
+      <c r="G190" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="191" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B191" s="3">
@@ -5387,7 +5646,9 @@
         <v>276</v>
       </c>
       <c r="F191" s="4"/>
-      <c r="G191" s="4"/>
+      <c r="G191" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="192" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B192" s="3">
@@ -5402,7 +5663,9 @@
         <v>294</v>
       </c>
       <c r="F192" s="13"/>
-      <c r="G192" s="4"/>
+      <c r="G192" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="193" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B193" s="15">
@@ -5417,7 +5680,9 @@
         <v>260</v>
       </c>
       <c r="F193" s="13"/>
-      <c r="G193" s="4"/>
+      <c r="G193" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="194" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B194" s="15">
@@ -5434,7 +5699,9 @@
         <v>8</v>
       </c>
       <c r="F194" s="13"/>
-      <c r="G194" s="4"/>
+      <c r="G194" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="195" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B195" s="2">
@@ -5463,7 +5730,9 @@
         <v>291</v>
       </c>
       <c r="F196" s="13"/>
-      <c r="G196" s="4"/>
+      <c r="G196" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="197" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B197" s="3">
@@ -5478,7 +5747,9 @@
         <v>294</v>
       </c>
       <c r="F197" s="13"/>
-      <c r="G197" s="4"/>
+      <c r="G197" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="198" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B198" s="3">
@@ -5493,14 +5764,16 @@
         <v>260</v>
       </c>
       <c r="F198" s="13"/>
-      <c r="G198" s="4"/>
+      <c r="G198" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="199" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B199" s="3">
         <f t="shared" si="11"/>
         <v>13.399999999999999</v>
       </c>
-      <c r="C199" s="54" t="s">
+      <c r="C199" s="47" t="s">
         <v>242</v>
       </c>
       <c r="D199" s="17" t="s">
@@ -5510,14 +5783,16 @@
         <v>297</v>
       </c>
       <c r="F199" s="13"/>
-      <c r="G199" s="4"/>
+      <c r="G199" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="200" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B200" s="3">
         <f t="shared" si="11"/>
         <v>13.499999999999998</v>
       </c>
-      <c r="C200" s="55"/>
+      <c r="C200" s="48"/>
       <c r="D200" s="17" t="s">
         <v>298</v>
       </c>
@@ -5527,14 +5802,16 @@
       <c r="F200" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="G200" s="4"/>
+      <c r="G200" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="201" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B201" s="3">
         <f t="shared" si="11"/>
         <v>13.599999999999998</v>
       </c>
-      <c r="C201" s="56"/>
+      <c r="C201" s="49"/>
       <c r="D201" s="17" t="s">
         <v>301</v>
       </c>
@@ -5542,7 +5819,9 @@
         <v>300</v>
       </c>
       <c r="F201" s="13"/>
-      <c r="G201" s="4"/>
+      <c r="G201" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="202" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B202" s="3">
@@ -5559,7 +5838,9 @@
         <v>307</v>
       </c>
       <c r="F202" s="13"/>
-      <c r="G202" s="4"/>
+      <c r="G202" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="203" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B203" s="3">
@@ -5576,7 +5857,9 @@
         <v>304</v>
       </c>
       <c r="F203" s="13"/>
-      <c r="G203" s="4"/>
+      <c r="G203" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="204" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B204" s="3">
@@ -5593,7 +5876,9 @@
         <v>309</v>
       </c>
       <c r="F204" s="13"/>
-      <c r="G204" s="4"/>
+      <c r="G204" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="205" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B205" s="15">
@@ -5610,7 +5895,9 @@
         <v>307</v>
       </c>
       <c r="F205" s="13"/>
-      <c r="G205" s="4"/>
+      <c r="G205" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="206" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B206" s="15">
@@ -5625,7 +5912,9 @@
         <v>279</v>
       </c>
       <c r="F206" s="4"/>
-      <c r="G206" s="4"/>
+      <c r="G206" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="207" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B207" s="15">
@@ -5642,7 +5931,9 @@
         <v>271</v>
       </c>
       <c r="F207" s="4"/>
-      <c r="G207" s="4"/>
+      <c r="G207" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="208" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B208" s="15">
@@ -5659,7 +5950,9 @@
         <v>281</v>
       </c>
       <c r="F208" s="4"/>
-      <c r="G208" s="4"/>
+      <c r="G208" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="209" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B209" s="15">
@@ -5676,7 +5969,9 @@
         <v>276</v>
       </c>
       <c r="F209" s="4"/>
-      <c r="G209" s="4"/>
+      <c r="G209" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="210" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B210" s="15">
@@ -5693,7 +5988,9 @@
         <v>8</v>
       </c>
       <c r="F210" s="4"/>
-      <c r="G210" s="4"/>
+      <c r="G210" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="211" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B211" s="2">
@@ -5712,7 +6009,7 @@
         <f>B211+0.1</f>
         <v>14.1</v>
       </c>
-      <c r="C212" s="46" t="s">
+      <c r="C212" s="51" t="s">
         <v>242</v>
       </c>
       <c r="D212" s="17" t="s">
@@ -5722,14 +6019,16 @@
         <v>250</v>
       </c>
       <c r="F212" s="13"/>
-      <c r="G212" s="48"/>
+      <c r="G212" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="213" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B213" s="3">
         <f t="shared" ref="B213:B220" si="13">B212+0.1</f>
         <v>14.2</v>
       </c>
-      <c r="C213" s="60"/>
+      <c r="C213" s="52"/>
       <c r="D213" s="24" t="s">
         <v>245</v>
       </c>
@@ -5737,14 +6036,14 @@
         <v>251</v>
       </c>
       <c r="F213" s="13"/>
-      <c r="G213" s="49"/>
+      <c r="G213" s="52"/>
     </row>
     <row r="214" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B214" s="3">
         <f t="shared" si="13"/>
         <v>14.299999999999999</v>
       </c>
-      <c r="C214" s="60"/>
+      <c r="C214" s="52"/>
       <c r="D214" s="17" t="s">
         <v>244</v>
       </c>
@@ -5754,14 +6053,14 @@
       <c r="F214" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="G214" s="49"/>
+      <c r="G214" s="52"/>
     </row>
     <row r="215" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B215" s="3">
         <f t="shared" si="13"/>
         <v>14.399999999999999</v>
       </c>
-      <c r="C215" s="60"/>
+      <c r="C215" s="52"/>
       <c r="D215" s="17" t="s">
         <v>246</v>
       </c>
@@ -5769,14 +6068,14 @@
         <v>252</v>
       </c>
       <c r="F215" s="13"/>
-      <c r="G215" s="49"/>
+      <c r="G215" s="52"/>
     </row>
     <row r="216" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B216" s="3">
         <f t="shared" si="13"/>
         <v>14.499999999999998</v>
       </c>
-      <c r="C216" s="47"/>
+      <c r="C216" s="53"/>
       <c r="D216" s="17" t="s">
         <v>247</v>
       </c>
@@ -5784,35 +6083,37 @@
         <v>252</v>
       </c>
       <c r="F216" s="13"/>
-      <c r="G216" s="50"/>
+      <c r="G216" s="53"/>
     </row>
     <row r="217" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B217" s="3">
         <f t="shared" si="13"/>
         <v>14.599999999999998</v>
       </c>
-      <c r="C217" s="46" t="s">
+      <c r="C217" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="D217" s="51"/>
+      <c r="D217" s="57"/>
       <c r="E217" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="F217" s="51"/>
-      <c r="G217" s="48"/>
+      <c r="F217" s="57"/>
+      <c r="G217" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="218" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B218" s="3">
         <f t="shared" si="13"/>
         <v>14.699999999999998</v>
       </c>
-      <c r="C218" s="47"/>
-      <c r="D218" s="52"/>
+      <c r="C218" s="53"/>
+      <c r="D218" s="59"/>
       <c r="E218" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="F218" s="52"/>
-      <c r="G218" s="50"/>
+      <c r="F218" s="59"/>
+      <c r="G218" s="53"/>
     </row>
     <row r="219" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B219" s="3">
@@ -5827,7 +6128,9 @@
         <v>258</v>
       </c>
       <c r="F219" s="13"/>
-      <c r="G219" s="4"/>
+      <c r="G219" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="220" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B220" s="3">
@@ -5842,7 +6145,7 @@
         <v>260</v>
       </c>
       <c r="F220" s="13"/>
-      <c r="G220" s="4"/>
+      <c r="G220" s="53"/>
     </row>
     <row r="221" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B221" s="15">
@@ -5857,7 +6160,9 @@
         <v>261</v>
       </c>
       <c r="F221" s="13"/>
-      <c r="G221" s="4"/>
+      <c r="G221" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="222" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B222" s="15">
@@ -5872,7 +6177,7 @@
         <v>263</v>
       </c>
       <c r="F222" s="13"/>
-      <c r="G222" s="4"/>
+      <c r="G222" s="53"/>
     </row>
     <row r="223" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B223" s="15">
@@ -5887,7 +6192,9 @@
         <v>266</v>
       </c>
       <c r="F223" s="13"/>
-      <c r="G223" s="4"/>
+      <c r="G223" s="51" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="224" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B224" s="15">
@@ -5902,7 +6209,7 @@
         <v>267</v>
       </c>
       <c r="F224" s="13"/>
-      <c r="G224" s="4"/>
+      <c r="G224" s="53"/>
     </row>
     <row r="225" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B225" s="15">
@@ -5919,7 +6226,9 @@
         <v>8</v>
       </c>
       <c r="F225" s="13"/>
-      <c r="G225" s="4"/>
+      <c r="G225" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="226" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B226" s="2">
@@ -5946,7 +6255,9 @@
         <v>365</v>
       </c>
       <c r="F227" s="13"/>
-      <c r="G227" s="4"/>
+      <c r="G227" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="228" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B228" s="3">
@@ -5961,7 +6272,9 @@
         <v>364</v>
       </c>
       <c r="F228" s="13"/>
-      <c r="G228" s="4"/>
+      <c r="G228" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="229" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B229" s="3">
@@ -5976,7 +6289,9 @@
         <v>363</v>
       </c>
       <c r="F229" s="13"/>
-      <c r="G229" s="4"/>
+      <c r="G229" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="230" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B230" s="3">
@@ -5991,7 +6306,9 @@
         <v>368</v>
       </c>
       <c r="F230" s="13"/>
-      <c r="G230" s="4"/>
+      <c r="G230" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="231" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B231" s="2">
@@ -6033,7 +6350,9 @@
         <v>366</v>
       </c>
       <c r="F233" s="13"/>
-      <c r="G233" s="4"/>
+      <c r="G233" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="234" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B234" s="3" t="str">
@@ -6050,7 +6369,9 @@
         <v>363</v>
       </c>
       <c r="F234" s="13"/>
-      <c r="G234" s="4"/>
+      <c r="G234" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="235" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B235" s="25">
@@ -6080,7 +6401,9 @@
         <v>373</v>
       </c>
       <c r="F236" s="13"/>
-      <c r="G236" s="4"/>
+      <c r="G236" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="237" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="str">
@@ -6097,7 +6420,9 @@
         <v>363</v>
       </c>
       <c r="F237" s="13"/>
-      <c r="G237" s="4"/>
+      <c r="G237" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="238" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B238" s="2">
@@ -6124,7 +6449,9 @@
         <v>379</v>
       </c>
       <c r="F239" s="13"/>
-      <c r="G239" s="4"/>
+      <c r="G239" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="240" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B240" s="3">
@@ -6139,7 +6466,9 @@
         <v>377</v>
       </c>
       <c r="F240" s="13"/>
-      <c r="G240" s="4"/>
+      <c r="G240" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="241" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B241" s="2">
@@ -6166,7 +6495,9 @@
         <v>383</v>
       </c>
       <c r="F242" s="13"/>
-      <c r="G242" s="4"/>
+      <c r="G242" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="243" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B243" s="3">
@@ -6181,7 +6512,9 @@
         <v>382</v>
       </c>
       <c r="F243" s="13"/>
-      <c r="G243" s="4"/>
+      <c r="G243" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="244" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B244" s="2">
@@ -6208,7 +6541,9 @@
         <v>384</v>
       </c>
       <c r="F245" s="13"/>
-      <c r="G245" s="4"/>
+      <c r="G245" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="246" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B246" s="3">
@@ -6223,7 +6558,9 @@
         <v>393</v>
       </c>
       <c r="F246" s="13"/>
-      <c r="G246" s="4"/>
+      <c r="G246" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="247" spans="2:7" ht="52.4" x14ac:dyDescent="0.25">
       <c r="B247" s="3">
@@ -6238,7 +6575,9 @@
         <v>386</v>
       </c>
       <c r="F247" s="13"/>
-      <c r="G247" s="4"/>
+      <c r="G247" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="248" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B248" s="3">
@@ -6253,7 +6592,9 @@
         <v>387</v>
       </c>
       <c r="F248" s="13"/>
-      <c r="G248" s="4"/>
+      <c r="G248" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="249" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B249" s="3">
@@ -6268,7 +6609,9 @@
         <v>389</v>
       </c>
       <c r="F249" s="13"/>
-      <c r="G249" s="4"/>
+      <c r="G249" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="250" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B250" s="3">
@@ -6283,7 +6626,9 @@
         <v>391</v>
       </c>
       <c r="F250" s="13"/>
-      <c r="G250" s="4"/>
+      <c r="G250" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="251" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B251" s="3">
@@ -6300,7 +6645,9 @@
         <v>8</v>
       </c>
       <c r="F251" s="13"/>
-      <c r="G251" s="4"/>
+      <c r="G251" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="252" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B252" s="2">
@@ -6327,7 +6674,9 @@
         <v>397</v>
       </c>
       <c r="F253" s="13"/>
-      <c r="G253" s="4"/>
+      <c r="G253" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="254" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B254" s="3">
@@ -6342,7 +6691,9 @@
         <v>399</v>
       </c>
       <c r="F254" s="13"/>
-      <c r="G254" s="4"/>
+      <c r="G254" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="255" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B255" s="3">
@@ -6357,7 +6708,9 @@
         <v>401</v>
       </c>
       <c r="F255" s="13"/>
-      <c r="G255" s="4"/>
+      <c r="G255" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="256" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B256" s="3">
@@ -6372,7 +6725,9 @@
         <v>403</v>
       </c>
       <c r="F256" s="13"/>
-      <c r="G256" s="4"/>
+      <c r="G256" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="257" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B257" s="3">
@@ -6389,7 +6744,9 @@
         <v>8</v>
       </c>
       <c r="F257" s="13"/>
-      <c r="G257" s="4"/>
+      <c r="G257" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="258" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B258" s="2">
@@ -6416,7 +6773,9 @@
         <v>406</v>
       </c>
       <c r="F259" s="13"/>
-      <c r="G259" s="4"/>
+      <c r="G259" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="260" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B260" s="3">
@@ -6431,7 +6790,9 @@
         <v>408</v>
       </c>
       <c r="F260" s="13"/>
-      <c r="G260" s="4"/>
+      <c r="G260" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="261" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B261" s="3">
@@ -6446,7 +6807,9 @@
         <v>410</v>
       </c>
       <c r="F261" s="13"/>
-      <c r="G261" s="4"/>
+      <c r="G261" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="262" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B262" s="3">
@@ -6463,7 +6826,9 @@
       <c r="F262" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G262" s="4"/>
+      <c r="G262" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="263" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B263" s="3">
@@ -6482,7 +6847,9 @@
       <c r="F263" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G263" s="4"/>
+      <c r="G263" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="264" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B264" s="3">
@@ -6499,7 +6866,9 @@
       <c r="F264" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G264" s="4"/>
+      <c r="G264" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="265" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B265" s="3">
@@ -6516,7 +6885,9 @@
       <c r="F265" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G265" s="4"/>
+      <c r="G265" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="266" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B266" s="3">
@@ -6533,7 +6904,9 @@
       <c r="F266" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G266" s="4"/>
+      <c r="G266" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="267" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B267" s="3">
@@ -6550,7 +6923,9 @@
       <c r="F267" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G267" s="4"/>
+      <c r="G267" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="268" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B268" s="15">
@@ -6567,7 +6942,9 @@
       <c r="F268" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G268" s="4"/>
+      <c r="G268" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="269" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B269" s="15">
@@ -6584,7 +6961,9 @@
       <c r="F269" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="G269" s="4"/>
+      <c r="G269" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="270" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B270" s="15">
@@ -6601,7 +6980,9 @@
         <v>8</v>
       </c>
       <c r="F270" s="13"/>
-      <c r="G270" s="4"/>
+      <c r="G270" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="271" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B271" s="2">
@@ -6628,7 +7009,9 @@
         <v>433</v>
       </c>
       <c r="F272" s="13"/>
-      <c r="G272" s="4"/>
+      <c r="G272" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="273" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B273" s="3">
@@ -6643,7 +7026,9 @@
         <v>435</v>
       </c>
       <c r="F273" s="13"/>
-      <c r="G273" s="4"/>
+      <c r="G273" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="274" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B274" s="3">
@@ -6658,7 +7043,9 @@
         <v>134</v>
       </c>
       <c r="F274" s="13"/>
-      <c r="G274" s="4"/>
+      <c r="G274" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="275" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B275" s="3">
@@ -6673,7 +7060,9 @@
         <v>430</v>
       </c>
       <c r="F275" s="13"/>
-      <c r="G275" s="4"/>
+      <c r="G275" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="276" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B276" s="3">
@@ -6688,7 +7077,9 @@
         <v>430</v>
       </c>
       <c r="F276" s="13"/>
-      <c r="G276" s="4"/>
+      <c r="G276" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="277" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B277" s="3">
@@ -6703,7 +7094,9 @@
         <v>431</v>
       </c>
       <c r="F277" s="13"/>
-      <c r="G277" s="4"/>
+      <c r="G277" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="278" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B278" s="3">
@@ -6718,7 +7111,9 @@
         <v>438</v>
       </c>
       <c r="F278" s="13"/>
-      <c r="G278" s="4"/>
+      <c r="G278" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="279" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B279" s="3">
@@ -6733,7 +7128,9 @@
         <v>440</v>
       </c>
       <c r="F279" s="13"/>
-      <c r="G279" s="4"/>
+      <c r="G279" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="280" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B280" s="3">
@@ -6748,7 +7145,9 @@
         <v>442</v>
       </c>
       <c r="F280" s="13"/>
-      <c r="G280" s="4"/>
+      <c r="G280" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="281" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B281" s="15">
@@ -6765,7 +7164,9 @@
         <v>8</v>
       </c>
       <c r="F281" s="13"/>
-      <c r="G281" s="4"/>
+      <c r="G281" s="4" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="282" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B282" s="31">
@@ -7832,29 +8233,33 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="C114:C116"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="C121:C123"/>
-    <mergeCell ref="C166:C169"/>
-    <mergeCell ref="C149:C152"/>
-    <mergeCell ref="C146:C148"/>
-    <mergeCell ref="C142:C145"/>
-    <mergeCell ref="E162:E164"/>
-    <mergeCell ref="F162:F164"/>
-    <mergeCell ref="G162:G164"/>
-    <mergeCell ref="G142:G145"/>
-    <mergeCell ref="E166:E169"/>
-    <mergeCell ref="F166:F169"/>
-    <mergeCell ref="G166:G169"/>
-    <mergeCell ref="E153:E156"/>
-    <mergeCell ref="F153:F156"/>
-    <mergeCell ref="G139:G141"/>
-    <mergeCell ref="G146:G148"/>
-    <mergeCell ref="F149:F152"/>
-    <mergeCell ref="G149:G152"/>
-    <mergeCell ref="C139:C141"/>
-    <mergeCell ref="E149:E152"/>
+  <mergeCells count="64">
+    <mergeCell ref="G219:G220"/>
+    <mergeCell ref="G221:G222"/>
+    <mergeCell ref="G223:G224"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="G212:G216"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="D217:D218"/>
+    <mergeCell ref="G217:G218"/>
+    <mergeCell ref="F217:F218"/>
+    <mergeCell ref="G174:G178"/>
+    <mergeCell ref="E170:E173"/>
+    <mergeCell ref="F170:F173"/>
+    <mergeCell ref="G170:G173"/>
+    <mergeCell ref="E174:E178"/>
+    <mergeCell ref="F174:F178"/>
+    <mergeCell ref="E124:E127"/>
+    <mergeCell ref="F124:F127"/>
+    <mergeCell ref="G124:G127"/>
+    <mergeCell ref="E128:E131"/>
+    <mergeCell ref="C212:C216"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="B174:B178"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="B166:B169"/>
+    <mergeCell ref="C174:C178"/>
+    <mergeCell ref="C170:C173"/>
     <mergeCell ref="G114:G116"/>
     <mergeCell ref="B128:B131"/>
     <mergeCell ref="B124:B127"/>
@@ -7871,29 +8276,28 @@
     <mergeCell ref="G128:G131"/>
     <mergeCell ref="G121:G123"/>
     <mergeCell ref="G117:G120"/>
-    <mergeCell ref="C212:C216"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="B174:B178"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="B166:B169"/>
-    <mergeCell ref="C174:C178"/>
-    <mergeCell ref="C170:C173"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="G212:G216"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="D217:D218"/>
-    <mergeCell ref="G217:G218"/>
-    <mergeCell ref="F217:F218"/>
-    <mergeCell ref="G174:G178"/>
-    <mergeCell ref="E170:E173"/>
-    <mergeCell ref="F170:F173"/>
-    <mergeCell ref="G170:G173"/>
-    <mergeCell ref="E174:E178"/>
-    <mergeCell ref="F174:F178"/>
-    <mergeCell ref="E124:E127"/>
-    <mergeCell ref="F124:F127"/>
-    <mergeCell ref="G124:G127"/>
-    <mergeCell ref="E128:E131"/>
+    <mergeCell ref="G139:G141"/>
+    <mergeCell ref="G146:G148"/>
+    <mergeCell ref="F149:F152"/>
+    <mergeCell ref="G149:G152"/>
+    <mergeCell ref="C139:C141"/>
+    <mergeCell ref="E149:E152"/>
+    <mergeCell ref="E162:E164"/>
+    <mergeCell ref="F162:F164"/>
+    <mergeCell ref="G162:G164"/>
+    <mergeCell ref="G142:G145"/>
+    <mergeCell ref="E166:E169"/>
+    <mergeCell ref="F166:F169"/>
+    <mergeCell ref="G166:G169"/>
+    <mergeCell ref="E153:E156"/>
+    <mergeCell ref="F153:F156"/>
+    <mergeCell ref="C114:C116"/>
+    <mergeCell ref="C117:C120"/>
+    <mergeCell ref="C121:C123"/>
+    <mergeCell ref="C166:C169"/>
+    <mergeCell ref="C149:C152"/>
+    <mergeCell ref="C146:C148"/>
+    <mergeCell ref="C142:C145"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"Deloy DB and fix some bug"
</commit_message>
<xml_diff>
--- a/documents/BaoCaoDot3+4/Testcase.xlsx
+++ b/documents/BaoCaoDot3+4/Testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\JavaScript\streamingmovie\documents\BaoCaoDot3+4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DB21E7-64CE-4288-B109-87E37E9FAF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC2DE6-98C8-4CD5-A1A7-1231C9F7F312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2110,21 +2110,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2136,17 +2136,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2157,11 +2154,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2577,8 +2577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="E174" sqref="E174:E178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.55" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4240,7 +4240,7 @@
         <f>B99 + 0.1</f>
         <v>8.1</v>
       </c>
-      <c r="C100" s="51" t="s">
+      <c r="C100" s="48" t="s">
         <v>324</v>
       </c>
       <c r="D100" s="17" t="s">
@@ -4259,7 +4259,7 @@
         <f t="shared" ref="B101:B108" si="3">B100 + 0.1</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="C101" s="53"/>
+      <c r="C101" s="49"/>
       <c r="D101" s="17" t="s">
         <v>332</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>208</v>
       </c>
       <c r="F114" s="13"/>
-      <c r="G114" s="51" t="s">
+      <c r="G114" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -4514,7 +4514,7 @@
         <v>208</v>
       </c>
       <c r="F115" s="13"/>
-      <c r="G115" s="52"/>
+      <c r="G115" s="50"/>
     </row>
     <row r="116" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
       <c r="B116" s="3">
@@ -4529,14 +4529,14 @@
         <v>209</v>
       </c>
       <c r="F116" s="13"/>
-      <c r="G116" s="53"/>
+      <c r="G116" s="49"/>
     </row>
     <row r="117" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B117" s="3">
         <f t="shared" si="4"/>
         <v>9.7999999999999972</v>
       </c>
-      <c r="C117" s="57" t="s">
+      <c r="C117" s="53" t="s">
         <v>159</v>
       </c>
       <c r="D117" s="17" t="s">
@@ -4546,7 +4546,7 @@
         <v>202</v>
       </c>
       <c r="F117" s="13"/>
-      <c r="G117" s="51" t="s">
+      <c r="G117" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -4555,7 +4555,7 @@
         <f t="shared" si="4"/>
         <v>9.8999999999999968</v>
       </c>
-      <c r="C118" s="57"/>
+      <c r="C118" s="53"/>
       <c r="D118" s="17" t="s">
         <v>165</v>
       </c>
@@ -4563,14 +4563,14 @@
         <v>203</v>
       </c>
       <c r="F118" s="13"/>
-      <c r="G118" s="52"/>
+      <c r="G118" s="50"/>
     </row>
     <row r="119" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B119" s="15">
         <f>B110</f>
         <v>9.1</v>
       </c>
-      <c r="C119" s="57"/>
+      <c r="C119" s="53"/>
       <c r="D119" s="17" t="s">
         <v>166</v>
       </c>
@@ -4578,14 +4578,14 @@
         <v>204</v>
       </c>
       <c r="F119" s="13"/>
-      <c r="G119" s="52"/>
+      <c r="G119" s="50"/>
     </row>
     <row r="120" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B120" s="15">
         <f>B119+0.01</f>
         <v>9.11</v>
       </c>
-      <c r="C120" s="57"/>
+      <c r="C120" s="53"/>
       <c r="D120" s="17" t="s">
         <v>168</v>
       </c>
@@ -4593,14 +4593,14 @@
         <v>205</v>
       </c>
       <c r="F120" s="13"/>
-      <c r="G120" s="53"/>
+      <c r="G120" s="49"/>
     </row>
     <row r="121" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B121" s="15">
         <f t="shared" ref="B121:B123" si="5">B120+0.01</f>
         <v>9.1199999999999992</v>
       </c>
-      <c r="C121" s="51" t="s">
+      <c r="C121" s="48" t="s">
         <v>158</v>
       </c>
       <c r="D121" s="17" t="s">
@@ -4610,7 +4610,7 @@
         <v>206</v>
       </c>
       <c r="F121" s="13"/>
-      <c r="G121" s="51" t="s">
+      <c r="G121" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -4619,7 +4619,7 @@
         <f t="shared" si="5"/>
         <v>9.129999999999999</v>
       </c>
-      <c r="C122" s="52"/>
+      <c r="C122" s="50"/>
       <c r="D122" s="17" t="s">
         <v>170</v>
       </c>
@@ -4627,14 +4627,14 @@
         <v>206</v>
       </c>
       <c r="F122" s="13"/>
-      <c r="G122" s="52"/>
+      <c r="G122" s="50"/>
     </row>
     <row r="123" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B123" s="15">
         <f t="shared" si="5"/>
         <v>9.1399999999999988</v>
       </c>
-      <c r="C123" s="53"/>
+      <c r="C123" s="49"/>
       <c r="D123" s="17" t="s">
         <v>171</v>
       </c>
@@ -4642,10 +4642,10 @@
         <v>207</v>
       </c>
       <c r="F123" s="13"/>
-      <c r="G123" s="53"/>
+      <c r="G123" s="49"/>
     </row>
     <row r="124" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B124" s="58">
+      <c r="B124" s="63">
         <f>B123+0.01</f>
         <v>9.1499999999999986</v>
       </c>
@@ -4655,46 +4655,46 @@
       <c r="D124" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E124" s="51" t="s">
+      <c r="E124" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="F124" s="48"/>
-      <c r="G124" s="51" t="s">
+      <c r="F124" s="51"/>
+      <c r="G124" s="48" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="125" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B125" s="59"/>
+      <c r="B125" s="64"/>
       <c r="C125" s="55"/>
       <c r="D125" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E125" s="52"/>
-      <c r="F125" s="49"/>
-      <c r="G125" s="52"/>
+      <c r="E125" s="50"/>
+      <c r="F125" s="57"/>
+      <c r="G125" s="50"/>
     </row>
     <row r="126" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B126" s="59"/>
+      <c r="B126" s="64"/>
       <c r="C126" s="55"/>
       <c r="D126" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E126" s="52"/>
-      <c r="F126" s="49"/>
-      <c r="G126" s="52"/>
+      <c r="E126" s="50"/>
+      <c r="F126" s="57"/>
+      <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B127" s="60"/>
+      <c r="B127" s="65"/>
       <c r="C127" s="56"/>
       <c r="D127" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E127" s="53"/>
-      <c r="F127" s="50"/>
-      <c r="G127" s="53"/>
+      <c r="E127" s="49"/>
+      <c r="F127" s="52"/>
+      <c r="G127" s="49"/>
     </row>
     <row r="128" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B128" s="58">
+      <c r="B128" s="63">
         <f>B124+0.01</f>
         <v>9.1599999999999984</v>
       </c>
@@ -4704,43 +4704,43 @@
       <c r="D128" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E128" s="51" t="s">
+      <c r="E128" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="F128" s="48"/>
-      <c r="G128" s="51" t="s">
+      <c r="F128" s="51"/>
+      <c r="G128" s="48" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="129" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B129" s="59"/>
+      <c r="B129" s="64"/>
       <c r="C129" s="55"/>
       <c r="D129" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E129" s="52"/>
-      <c r="F129" s="49"/>
-      <c r="G129" s="52"/>
+      <c r="E129" s="50"/>
+      <c r="F129" s="57"/>
+      <c r="G129" s="50"/>
     </row>
     <row r="130" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B130" s="59"/>
+      <c r="B130" s="64"/>
       <c r="C130" s="55"/>
       <c r="D130" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E130" s="52"/>
-      <c r="F130" s="49"/>
-      <c r="G130" s="52"/>
+      <c r="E130" s="50"/>
+      <c r="F130" s="57"/>
+      <c r="G130" s="50"/>
     </row>
     <row r="131" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B131" s="60"/>
+      <c r="B131" s="65"/>
       <c r="C131" s="56"/>
       <c r="D131" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="E131" s="53"/>
-      <c r="F131" s="50"/>
-      <c r="G131" s="53"/>
+      <c r="E131" s="49"/>
+      <c r="F131" s="52"/>
+      <c r="G131" s="49"/>
     </row>
     <row r="132" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B132" s="15">
@@ -4867,7 +4867,7 @@
         <f t="shared" si="6"/>
         <v>10.499999999999998</v>
       </c>
-      <c r="C139" s="51" t="s">
+      <c r="C139" s="48" t="s">
         <v>160</v>
       </c>
       <c r="D139" s="17" t="s">
@@ -4877,7 +4877,7 @@
         <v>208</v>
       </c>
       <c r="F139" s="13"/>
-      <c r="G139" s="51" t="s">
+      <c r="G139" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -4886,7 +4886,7 @@
         <f t="shared" si="6"/>
         <v>10.599999999999998</v>
       </c>
-      <c r="C140" s="52"/>
+      <c r="C140" s="50"/>
       <c r="D140" s="17" t="s">
         <v>183</v>
       </c>
@@ -4894,14 +4894,14 @@
         <v>208</v>
       </c>
       <c r="F140" s="13"/>
-      <c r="G140" s="52"/>
+      <c r="G140" s="50"/>
     </row>
     <row r="141" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B141" s="3">
         <f t="shared" si="6"/>
         <v>10.699999999999998</v>
       </c>
-      <c r="C141" s="53"/>
+      <c r="C141" s="49"/>
       <c r="D141" s="17" t="s">
         <v>184</v>
       </c>
@@ -4909,14 +4909,14 @@
         <v>208</v>
       </c>
       <c r="F141" s="13"/>
-      <c r="G141" s="53"/>
+      <c r="G141" s="49"/>
     </row>
     <row r="142" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B142" s="3">
         <f t="shared" si="6"/>
         <v>10.799999999999997</v>
       </c>
-      <c r="C142" s="51" t="s">
+      <c r="C142" s="48" t="s">
         <v>159</v>
       </c>
       <c r="D142" s="17" t="s">
@@ -4926,7 +4926,7 @@
         <v>212</v>
       </c>
       <c r="F142" s="13"/>
-      <c r="G142" s="51" t="s">
+      <c r="G142" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -4935,7 +4935,7 @@
         <f t="shared" si="6"/>
         <v>10.899999999999997</v>
       </c>
-      <c r="C143" s="52"/>
+      <c r="C143" s="50"/>
       <c r="D143" s="17" t="s">
         <v>185</v>
       </c>
@@ -4943,14 +4943,14 @@
         <v>213</v>
       </c>
       <c r="F143" s="13"/>
-      <c r="G143" s="52"/>
+      <c r="G143" s="50"/>
     </row>
     <row r="144" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B144" s="15">
         <f>B135</f>
         <v>10.1</v>
       </c>
-      <c r="C144" s="52"/>
+      <c r="C144" s="50"/>
       <c r="D144" s="17" t="s">
         <v>166</v>
       </c>
@@ -4958,14 +4958,14 @@
         <v>204</v>
       </c>
       <c r="F144" s="13"/>
-      <c r="G144" s="52"/>
+      <c r="G144" s="50"/>
     </row>
     <row r="145" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B145" s="15">
         <f>B144+0.01</f>
         <v>10.11</v>
       </c>
-      <c r="C145" s="53"/>
+      <c r="C145" s="49"/>
       <c r="D145" s="17" t="s">
         <v>168</v>
       </c>
@@ -4973,14 +4973,14 @@
         <v>205</v>
       </c>
       <c r="F145" s="13"/>
-      <c r="G145" s="53"/>
+      <c r="G145" s="49"/>
     </row>
     <row r="146" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B146" s="15">
         <f t="shared" ref="B146:B149" si="7">B145+0.01</f>
         <v>10.119999999999999</v>
       </c>
-      <c r="C146" s="51" t="s">
+      <c r="C146" s="48" t="s">
         <v>158</v>
       </c>
       <c r="D146" s="17" t="s">
@@ -4990,7 +4990,7 @@
         <v>206</v>
       </c>
       <c r="F146" s="13"/>
-      <c r="G146" s="51" t="s">
+      <c r="G146" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -4999,7 +4999,7 @@
         <f t="shared" si="7"/>
         <v>10.129999999999999</v>
       </c>
-      <c r="C147" s="52"/>
+      <c r="C147" s="50"/>
       <c r="D147" s="17" t="s">
         <v>170</v>
       </c>
@@ -5007,14 +5007,14 @@
         <v>206</v>
       </c>
       <c r="F147" s="13"/>
-      <c r="G147" s="52"/>
+      <c r="G147" s="50"/>
     </row>
     <row r="148" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B148" s="15">
         <f t="shared" si="7"/>
         <v>10.139999999999999</v>
       </c>
-      <c r="C148" s="53"/>
+      <c r="C148" s="49"/>
       <c r="D148" s="17" t="s">
         <v>171</v>
       </c>
@@ -5022,10 +5022,10 @@
         <v>214</v>
       </c>
       <c r="F148" s="13"/>
-      <c r="G148" s="53"/>
+      <c r="G148" s="49"/>
     </row>
     <row r="149" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B149" s="58">
+      <c r="B149" s="63">
         <f t="shared" si="7"/>
         <v>10.149999999999999</v>
       </c>
@@ -5035,46 +5035,46 @@
       <c r="D149" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E149" s="51" t="s">
+      <c r="E149" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="F149" s="48"/>
-      <c r="G149" s="51" t="s">
+      <c r="F149" s="51"/>
+      <c r="G149" s="48" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="150" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B150" s="59"/>
+      <c r="B150" s="64"/>
       <c r="C150" s="55"/>
       <c r="D150" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E150" s="52"/>
-      <c r="F150" s="49"/>
-      <c r="G150" s="52"/>
+      <c r="E150" s="50"/>
+      <c r="F150" s="57"/>
+      <c r="G150" s="50"/>
     </row>
     <row r="151" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B151" s="59"/>
+      <c r="B151" s="64"/>
       <c r="C151" s="55"/>
       <c r="D151" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E151" s="52"/>
-      <c r="F151" s="49"/>
-      <c r="G151" s="52"/>
+      <c r="E151" s="50"/>
+      <c r="F151" s="57"/>
+      <c r="G151" s="50"/>
     </row>
     <row r="152" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B152" s="60"/>
+      <c r="B152" s="65"/>
       <c r="C152" s="56"/>
       <c r="D152" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="E152" s="53"/>
-      <c r="F152" s="50"/>
-      <c r="G152" s="53"/>
+      <c r="E152" s="49"/>
+      <c r="F152" s="52"/>
+      <c r="G152" s="49"/>
     </row>
     <row r="153" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B153" s="58">
+      <c r="B153" s="63">
         <f>B149+0.01</f>
         <v>10.159999999999998</v>
       </c>
@@ -5084,43 +5084,43 @@
       <c r="D153" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="E153" s="51" t="s">
+      <c r="E153" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="F153" s="48"/>
-      <c r="G153" s="51" t="s">
+      <c r="F153" s="51"/>
+      <c r="G153" s="48" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="154" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B154" s="62"/>
+      <c r="B154" s="61"/>
       <c r="C154" s="55"/>
       <c r="D154" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E154" s="52"/>
-      <c r="F154" s="49"/>
-      <c r="G154" s="52"/>
+      <c r="E154" s="50"/>
+      <c r="F154" s="57"/>
+      <c r="G154" s="50"/>
     </row>
     <row r="155" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B155" s="62"/>
+      <c r="B155" s="61"/>
       <c r="C155" s="55"/>
       <c r="D155" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E155" s="52"/>
-      <c r="F155" s="49"/>
-      <c r="G155" s="52"/>
+      <c r="E155" s="50"/>
+      <c r="F155" s="57"/>
+      <c r="G155" s="50"/>
     </row>
     <row r="156" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B156" s="63"/>
+      <c r="B156" s="62"/>
       <c r="C156" s="56"/>
       <c r="D156" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="E156" s="53"/>
-      <c r="F156" s="50"/>
-      <c r="G156" s="53"/>
+      <c r="E156" s="49"/>
+      <c r="F156" s="52"/>
+      <c r="G156" s="49"/>
     </row>
     <row r="157" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B157" s="15">
@@ -5215,45 +5215,45 @@
       </c>
     </row>
     <row r="162" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
-      <c r="B162" s="61">
+      <c r="B162" s="60">
         <f>B161+0.1</f>
         <v>11.299999999999999</v>
       </c>
-      <c r="C162" s="51" t="s">
+      <c r="C162" s="48" t="s">
         <v>192</v>
       </c>
       <c r="D162" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E162" s="51" t="s">
+      <c r="E162" s="48" t="s">
         <v>194</v>
       </c>
       <c r="F162" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="G162" s="51" t="s">
+      <c r="G162" s="48" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="163" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
-      <c r="B163" s="62"/>
-      <c r="C163" s="52"/>
+      <c r="B163" s="61"/>
+      <c r="C163" s="50"/>
       <c r="D163" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E163" s="52"/>
+      <c r="E163" s="50"/>
       <c r="F163" s="55"/>
-      <c r="G163" s="52"/>
+      <c r="G163" s="50"/>
     </row>
     <row r="164" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
-      <c r="B164" s="63"/>
-      <c r="C164" s="53"/>
+      <c r="B164" s="62"/>
+      <c r="C164" s="49"/>
       <c r="D164" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="E164" s="53"/>
+      <c r="E164" s="49"/>
       <c r="F164" s="56"/>
-      <c r="G164" s="53"/>
+      <c r="G164" s="49"/>
     </row>
     <row r="165" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B165" s="3">
@@ -5277,60 +5277,60 @@
       </c>
     </row>
     <row r="166" spans="2:7" ht="39.299999999999997" x14ac:dyDescent="0.25">
-      <c r="B166" s="61">
+      <c r="B166" s="60">
         <f>B165+0.1</f>
         <v>11.499999999999998</v>
       </c>
-      <c r="C166" s="51" t="s">
+      <c r="C166" s="48" t="s">
         <v>219</v>
       </c>
       <c r="D166" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="E166" s="51" t="s">
+      <c r="E166" s="48" t="s">
         <v>224</v>
       </c>
-      <c r="F166" s="48"/>
-      <c r="G166" s="51" t="s">
+      <c r="F166" s="51"/>
+      <c r="G166" s="48" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="167" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B167" s="62"/>
-      <c r="C167" s="52"/>
+      <c r="B167" s="61"/>
+      <c r="C167" s="50"/>
       <c r="D167" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E167" s="52"/>
-      <c r="F167" s="49"/>
-      <c r="G167" s="52"/>
+      <c r="E167" s="50"/>
+      <c r="F167" s="57"/>
+      <c r="G167" s="50"/>
     </row>
     <row r="168" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B168" s="62"/>
-      <c r="C168" s="52"/>
+      <c r="B168" s="61"/>
+      <c r="C168" s="50"/>
       <c r="D168" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E168" s="52"/>
-      <c r="F168" s="49"/>
-      <c r="G168" s="52"/>
+      <c r="E168" s="50"/>
+      <c r="F168" s="57"/>
+      <c r="G168" s="50"/>
     </row>
     <row r="169" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
-      <c r="B169" s="63"/>
-      <c r="C169" s="53"/>
+      <c r="B169" s="62"/>
+      <c r="C169" s="49"/>
       <c r="D169" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="E169" s="53"/>
-      <c r="F169" s="50"/>
-      <c r="G169" s="53"/>
+      <c r="E169" s="49"/>
+      <c r="F169" s="52"/>
+      <c r="G169" s="49"/>
     </row>
     <row r="170" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B170" s="61">
+      <c r="B170" s="60">
         <f>B166+0.1</f>
         <v>11.599999999999998</v>
       </c>
-      <c r="C170" s="51" t="s">
+      <c r="C170" s="48" t="s">
         <v>231</v>
       </c>
       <c r="D170" s="17" t="s">
@@ -5339,99 +5339,99 @@
       <c r="E170" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="F170" s="48"/>
-      <c r="G170" s="51" t="s">
+      <c r="F170" s="51"/>
+      <c r="G170" s="48" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="171" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B171" s="62"/>
-      <c r="C171" s="52"/>
+      <c r="B171" s="61"/>
+      <c r="C171" s="50"/>
       <c r="D171" s="17" t="s">
         <v>220</v>
       </c>
       <c r="E171" s="55"/>
-      <c r="F171" s="49"/>
-      <c r="G171" s="52"/>
+      <c r="F171" s="57"/>
+      <c r="G171" s="50"/>
     </row>
     <row r="172" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B172" s="62"/>
-      <c r="C172" s="52"/>
+      <c r="B172" s="61"/>
+      <c r="C172" s="50"/>
       <c r="D172" s="7" t="s">
         <v>232</v>
       </c>
       <c r="E172" s="55"/>
-      <c r="F172" s="49"/>
-      <c r="G172" s="52"/>
+      <c r="F172" s="57"/>
+      <c r="G172" s="50"/>
     </row>
     <row r="173" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B173" s="63"/>
-      <c r="C173" s="53"/>
+      <c r="B173" s="62"/>
+      <c r="C173" s="49"/>
       <c r="D173" s="7" t="s">
         <v>233</v>
       </c>
       <c r="E173" s="56"/>
-      <c r="F173" s="50"/>
-      <c r="G173" s="53"/>
+      <c r="F173" s="52"/>
+      <c r="G173" s="49"/>
     </row>
     <row r="174" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B174" s="61">
+      <c r="B174" s="60">
         <f>B170+0.1</f>
         <v>11.699999999999998</v>
       </c>
-      <c r="C174" s="64" t="s">
+      <c r="C174" s="58" t="s">
         <v>235</v>
       </c>
       <c r="D174" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="E174" s="64" t="s">
+      <c r="E174" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="F174" s="65"/>
-      <c r="G174" s="57" t="s">
+      <c r="F174" s="59"/>
+      <c r="G174" s="53" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="175" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B175" s="62"/>
-      <c r="C175" s="64"/>
+      <c r="B175" s="61"/>
+      <c r="C175" s="58"/>
       <c r="D175" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="E175" s="64"/>
-      <c r="F175" s="65"/>
-      <c r="G175" s="57"/>
+      <c r="E175" s="58"/>
+      <c r="F175" s="59"/>
+      <c r="G175" s="53"/>
     </row>
     <row r="176" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B176" s="62"/>
-      <c r="C176" s="64"/>
+      <c r="B176" s="61"/>
+      <c r="C176" s="58"/>
       <c r="D176" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="E176" s="64"/>
-      <c r="F176" s="65"/>
-      <c r="G176" s="57"/>
+      <c r="E176" s="58"/>
+      <c r="F176" s="59"/>
+      <c r="G176" s="53"/>
     </row>
     <row r="177" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B177" s="62"/>
-      <c r="C177" s="64"/>
+      <c r="B177" s="61"/>
+      <c r="C177" s="58"/>
       <c r="D177" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="E177" s="64"/>
-      <c r="F177" s="65"/>
-      <c r="G177" s="57"/>
+      <c r="E177" s="58"/>
+      <c r="F177" s="59"/>
+      <c r="G177" s="53"/>
     </row>
     <row r="178" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
-      <c r="B178" s="63"/>
-      <c r="C178" s="64"/>
+      <c r="B178" s="62"/>
+      <c r="C178" s="58"/>
       <c r="D178" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="E178" s="64"/>
-      <c r="F178" s="65"/>
-      <c r="G178" s="57"/>
+      <c r="E178" s="58"/>
+      <c r="F178" s="59"/>
+      <c r="G178" s="53"/>
     </row>
     <row r="179" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B179" s="3">
@@ -5455,7 +5455,7 @@
         <f>B179+0.1</f>
         <v>11.899999999999997</v>
       </c>
-      <c r="C180" s="51" t="s">
+      <c r="C180" s="48" t="s">
         <v>178</v>
       </c>
       <c r="D180" s="17" t="s">
@@ -5474,7 +5474,7 @@
         <f>B160</f>
         <v>11.1</v>
       </c>
-      <c r="C181" s="53"/>
+      <c r="C181" s="49"/>
       <c r="D181" s="17" t="s">
         <v>181</v>
       </c>
@@ -6035,7 +6035,7 @@
         <f>B212+0.1</f>
         <v>14.1</v>
       </c>
-      <c r="C213" s="51" t="s">
+      <c r="C213" s="48" t="s">
         <v>242</v>
       </c>
       <c r="D213" s="17" t="s">
@@ -6045,7 +6045,7 @@
         <v>250</v>
       </c>
       <c r="F213" s="13"/>
-      <c r="G213" s="51" t="s">
+      <c r="G213" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6054,7 +6054,7 @@
         <f t="shared" ref="B214:B221" si="13">B213+0.1</f>
         <v>14.2</v>
       </c>
-      <c r="C214" s="52"/>
+      <c r="C214" s="50"/>
       <c r="D214" s="24" t="s">
         <v>245</v>
       </c>
@@ -6062,14 +6062,14 @@
         <v>251</v>
       </c>
       <c r="F214" s="13"/>
-      <c r="G214" s="52"/>
+      <c r="G214" s="50"/>
     </row>
     <row r="215" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B215" s="3">
         <f t="shared" si="13"/>
         <v>14.299999999999999</v>
       </c>
-      <c r="C215" s="52"/>
+      <c r="C215" s="50"/>
       <c r="D215" s="17" t="s">
         <v>244</v>
       </c>
@@ -6079,14 +6079,14 @@
       <c r="F215" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="G215" s="52"/>
+      <c r="G215" s="50"/>
     </row>
     <row r="216" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B216" s="3">
         <f t="shared" si="13"/>
         <v>14.399999999999999</v>
       </c>
-      <c r="C216" s="52"/>
+      <c r="C216" s="50"/>
       <c r="D216" s="17" t="s">
         <v>246</v>
       </c>
@@ -6094,14 +6094,14 @@
         <v>252</v>
       </c>
       <c r="F216" s="13"/>
-      <c r="G216" s="52"/>
+      <c r="G216" s="50"/>
     </row>
     <row r="217" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B217" s="3">
         <f t="shared" si="13"/>
         <v>14.499999999999998</v>
       </c>
-      <c r="C217" s="53"/>
+      <c r="C217" s="49"/>
       <c r="D217" s="17" t="s">
         <v>247</v>
       </c>
@@ -6109,22 +6109,22 @@
         <v>252</v>
       </c>
       <c r="F217" s="13"/>
-      <c r="G217" s="53"/>
+      <c r="G217" s="49"/>
     </row>
     <row r="218" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B218" s="3">
         <f t="shared" si="13"/>
         <v>14.599999999999998</v>
       </c>
-      <c r="C218" s="51" t="s">
+      <c r="C218" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="D218" s="48"/>
+      <c r="D218" s="51"/>
       <c r="E218" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="F218" s="48"/>
-      <c r="G218" s="51" t="s">
+      <c r="F218" s="51"/>
+      <c r="G218" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6133,13 +6133,13 @@
         <f t="shared" si="13"/>
         <v>14.699999999999998</v>
       </c>
-      <c r="C219" s="53"/>
-      <c r="D219" s="50"/>
+      <c r="C219" s="49"/>
+      <c r="D219" s="52"/>
       <c r="E219" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="F219" s="50"/>
-      <c r="G219" s="53"/>
+      <c r="F219" s="52"/>
+      <c r="G219" s="49"/>
     </row>
     <row r="220" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B220" s="3">
@@ -6154,7 +6154,7 @@
         <v>258</v>
       </c>
       <c r="F220" s="13"/>
-      <c r="G220" s="51" t="s">
+      <c r="G220" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6171,7 +6171,7 @@
         <v>260</v>
       </c>
       <c r="F221" s="13"/>
-      <c r="G221" s="53"/>
+      <c r="G221" s="49"/>
     </row>
     <row r="222" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B222" s="15">
@@ -6186,7 +6186,7 @@
         <v>261</v>
       </c>
       <c r="F222" s="13"/>
-      <c r="G222" s="51" t="s">
+      <c r="G222" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6203,7 +6203,7 @@
         <v>263</v>
       </c>
       <c r="F223" s="13"/>
-      <c r="G223" s="53"/>
+      <c r="G223" s="49"/>
     </row>
     <row r="224" spans="2:7" ht="26.2" x14ac:dyDescent="0.25">
       <c r="B224" s="15">
@@ -6218,7 +6218,7 @@
         <v>266</v>
       </c>
       <c r="F224" s="13"/>
-      <c r="G224" s="51" t="s">
+      <c r="G224" s="48" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6235,7 +6235,7 @@
         <v>267</v>
       </c>
       <c r="F225" s="13"/>
-      <c r="G225" s="53"/>
+      <c r="G225" s="49"/>
     </row>
     <row r="226" spans="2:7" ht="13.1" x14ac:dyDescent="0.25">
       <c r="B226" s="15">
@@ -8260,6 +8260,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="F166:F169"/>
+    <mergeCell ref="G166:G169"/>
+    <mergeCell ref="E153:E156"/>
+    <mergeCell ref="F153:F156"/>
+    <mergeCell ref="C114:C116"/>
+    <mergeCell ref="C117:C120"/>
+    <mergeCell ref="C121:C123"/>
+    <mergeCell ref="C166:C169"/>
+    <mergeCell ref="C149:C152"/>
+    <mergeCell ref="C146:C148"/>
+    <mergeCell ref="C142:C145"/>
+    <mergeCell ref="G114:G116"/>
+    <mergeCell ref="G153:G156"/>
+    <mergeCell ref="F128:F131"/>
+    <mergeCell ref="G128:G131"/>
+    <mergeCell ref="G121:G123"/>
+    <mergeCell ref="G117:G120"/>
+    <mergeCell ref="B174:B178"/>
+    <mergeCell ref="B170:B173"/>
+    <mergeCell ref="B166:B169"/>
+    <mergeCell ref="C174:C178"/>
+    <mergeCell ref="C170:C173"/>
+    <mergeCell ref="F124:F127"/>
+    <mergeCell ref="G124:G127"/>
+    <mergeCell ref="E128:E131"/>
+    <mergeCell ref="B128:B131"/>
+    <mergeCell ref="B124:B127"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B153:B156"/>
+    <mergeCell ref="B149:B152"/>
+    <mergeCell ref="C124:C127"/>
+    <mergeCell ref="C128:C131"/>
+    <mergeCell ref="C213:C217"/>
+    <mergeCell ref="C200:C202"/>
+    <mergeCell ref="G139:G141"/>
+    <mergeCell ref="G146:G148"/>
+    <mergeCell ref="F149:F152"/>
+    <mergeCell ref="G149:G152"/>
+    <mergeCell ref="C139:C141"/>
+    <mergeCell ref="E149:E152"/>
+    <mergeCell ref="E162:E164"/>
+    <mergeCell ref="F162:F164"/>
+    <mergeCell ref="G162:G164"/>
+    <mergeCell ref="G142:G145"/>
+    <mergeCell ref="E166:E169"/>
+    <mergeCell ref="C180:C181"/>
+    <mergeCell ref="C153:C156"/>
+    <mergeCell ref="C162:C164"/>
     <mergeCell ref="G220:G221"/>
     <mergeCell ref="G222:G223"/>
     <mergeCell ref="G224:G225"/>
@@ -8276,54 +8324,6 @@
     <mergeCell ref="E174:E178"/>
     <mergeCell ref="F174:F178"/>
     <mergeCell ref="E124:E127"/>
-    <mergeCell ref="C213:C217"/>
-    <mergeCell ref="C200:C202"/>
-    <mergeCell ref="G139:G141"/>
-    <mergeCell ref="G146:G148"/>
-    <mergeCell ref="F149:F152"/>
-    <mergeCell ref="G149:G152"/>
-    <mergeCell ref="C139:C141"/>
-    <mergeCell ref="E149:E152"/>
-    <mergeCell ref="E162:E164"/>
-    <mergeCell ref="F162:F164"/>
-    <mergeCell ref="G162:G164"/>
-    <mergeCell ref="G142:G145"/>
-    <mergeCell ref="E166:E169"/>
-    <mergeCell ref="G117:G120"/>
-    <mergeCell ref="B174:B178"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="B166:B169"/>
-    <mergeCell ref="C174:C178"/>
-    <mergeCell ref="C170:C173"/>
-    <mergeCell ref="F124:F127"/>
-    <mergeCell ref="G124:G127"/>
-    <mergeCell ref="E128:E131"/>
-    <mergeCell ref="B128:B131"/>
-    <mergeCell ref="B124:B127"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="C180:C181"/>
-    <mergeCell ref="B153:B156"/>
-    <mergeCell ref="B149:B152"/>
-    <mergeCell ref="C124:C127"/>
-    <mergeCell ref="C128:C131"/>
-    <mergeCell ref="C153:C156"/>
-    <mergeCell ref="C162:C164"/>
-    <mergeCell ref="F166:F169"/>
-    <mergeCell ref="G166:G169"/>
-    <mergeCell ref="E153:E156"/>
-    <mergeCell ref="F153:F156"/>
-    <mergeCell ref="C114:C116"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="C121:C123"/>
-    <mergeCell ref="C166:C169"/>
-    <mergeCell ref="C149:C152"/>
-    <mergeCell ref="C146:C148"/>
-    <mergeCell ref="C142:C145"/>
-    <mergeCell ref="G114:G116"/>
-    <mergeCell ref="G153:G156"/>
-    <mergeCell ref="F128:F131"/>
-    <mergeCell ref="G128:G131"/>
-    <mergeCell ref="G121:G123"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>